<commit_message>
Config file changed and eports files added in report section
</commit_message>
<xml_diff>
--- a/src/main/resources/date_SALT_Test_Data.xlsx
+++ b/src/main/resources/date_SALT_Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15855" windowHeight="6180" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15855" windowHeight="6180" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="RTS100_DATE" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7155" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7165" uniqueCount="1019">
   <si>
     <t>Line_Number</t>
   </si>
@@ -3080,6 +3080,9 @@
   </si>
   <si>
     <t>08/16/1983</t>
+  </si>
+  <si>
+    <t>08/23/1686</t>
   </si>
 </sst>
 </file>
@@ -13783,9 +13786,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L401"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H176" sqref="H176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28736,9 +28739,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28823,6 +28828,41 @@
       </c>
       <c r="K2" s="2" t="s">
         <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>173</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>